<commit_message>
change excel column 11 to bool
</commit_message>
<xml_diff>
--- a/dataset_2022/big_skill_by_Vitas.xlsx
+++ b/dataset_2022/big_skill_by_Vitas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="100">
   <si>
     <t xml:space="preserve">ASIN</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t xml:space="preserve">{'en-AU': 'English (AU)', 'en-CA': 'English (CA)', 'en-GB': 'English (GB)', 'en-IN': 'English (IN)', 'en-US': 'English (US)'}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">{'en-IN': 'song quiz', 'en-AU': 'song quiz', 'en-US': 'song quiz', 'en-CA': 'song quiz', 'en-GB': 'song quiz'}</t>
@@ -727,7 +730,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -736,11 +739,15 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -828,11 +835,11 @@
   </sheetPr>
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="7:7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
@@ -906,428 +913,428 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="P2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="Q2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="R2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="S2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="T2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="0" t="s">
+      <c r="U2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="V2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="W2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="2" t="n">
         <v>2.3</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="2" t="n">
         <v>18297</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" s="0" t="s">
+      <c r="L3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="M3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="N3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="O3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="P3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="Q3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="S3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="0" t="s">
+      <c r="T3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="V3" s="0" t="s">
+      <c r="U3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="W3" s="0" t="s">
-        <v>35</v>
+      <c r="V3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="0" t="s">
+    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="0" t="n">
+      <c r="B4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>3.4</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="0" t="s">
+      <c r="H4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="I4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="J4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M4" s="0" t="s">
+      <c r="K4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="L4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" s="4" t="s">
+      <c r="N4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="O4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="0" t="s">
+      <c r="Q4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="S4" s="0" t="s">
+      <c r="R4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="0" t="s">
+      <c r="S4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="U4" s="0" t="s">
+      <c r="T4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="V4" s="0" t="s">
+      <c r="U4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="W4" s="0" t="s">
+      <c r="V4" s="2" t="s">
         <v>55</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="C5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="2" t="n">
         <v>4.1</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="2" t="n">
         <v>8684</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="I5" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="J5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="L5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" s="0" t="s">
+      <c r="K5" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N5" s="0" t="s">
+      <c r="L5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O5" s="0" t="s">
+      <c r="N5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="O5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q5" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="S5" s="0" t="s">
+      <c r="P5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="T5" s="0" t="s">
+      <c r="Q5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="U5" s="0" t="s">
+      <c r="T5" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="V5" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="W5" s="0" t="s">
-        <v>35</v>
+      <c r="U5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="0" t="s">
+    <row r="6" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="C6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="2" t="n">
         <v>2.7</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H6" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="I6" s="0" t="s">
+      <c r="H6" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="I6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="J6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="3" t="b">
+      <c r="L6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M6" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="N6" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q6" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="R6" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="S6" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="T6" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="U6" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="V6" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="W6" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="126.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="0" t="n">
+      <c r="E7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H7" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="I7" s="0" t="s">
+      <c r="H7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J7" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="K7" s="0" t="s">
+      <c r="I7" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M7" s="0" t="s">
+      <c r="J7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="N7" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" s="4" t="s">
+      <c r="L7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="N7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="R7" s="0" t="s">
+      <c r="Q7" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="S7" s="0" t="s">
+      <c r="R7" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="T7" s="0" t="s">
+      <c r="S7" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="U7" s="0" t="s">
+      <c r="T7" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="V7" s="0" t="s">
+      <c r="U7" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="W7" s="0" t="s">
+      <c r="V7" s="2" t="s">
         <v>98</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>